<commit_message>
alter debug for de-rating
</commit_message>
<xml_diff>
--- a/test files/Tesla Model 3 PV LIMITS.xlsx
+++ b/test files/Tesla Model 3 PV LIMITS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>B1</t>
   </si>
@@ -111,9 +111,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>50C</t>
-  </si>
-  <si>
     <t>B sample</t>
   </si>
   <si>
@@ -129,12 +126,6 @@
     <t>Stop SAE</t>
   </si>
   <si>
-    <t>95C</t>
-  </si>
-  <si>
-    <t>50C, 60C, 95C =&gt; use 85C limits</t>
-  </si>
-  <si>
     <t>Reverse</t>
   </si>
   <si>
@@ -154,6 +145,18 @@
   </si>
   <si>
     <t>8J Reverse</t>
+  </si>
+  <si>
+    <t>45C</t>
+  </si>
+  <si>
+    <t>70C</t>
+  </si>
+  <si>
+    <t>60C, 95C =&gt; use 85C limits</t>
+  </si>
+  <si>
+    <t>45C =&gt; use 23C limits</t>
   </si>
 </sst>
 </file>
@@ -449,6 +452,13 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -467,6 +477,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -493,16 +506,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,8 +797,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +812,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -817,7 +820,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -837,7 +840,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>6</v>
@@ -852,7 +855,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="19"/>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="32" t="s">
         <v>26</v>
       </c>
       <c r="K4" s="10" t="s">
@@ -867,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>18</v>
@@ -886,7 +889,7 @@
         <v>21</v>
       </c>
       <c r="I5" s="20"/>
-      <c r="J5" s="29"/>
+      <c r="J5" s="32"/>
       <c r="K5" s="23">
         <v>0</v>
       </c>
@@ -899,15 +902,15 @@
         <v>1</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="13" t="s">
@@ -927,13 +930,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="31"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="13" t="s">
         <v>21</v>
       </c>
@@ -951,13 +954,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="32"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="13" t="s">
         <v>21</v>
       </c>
@@ -976,13 +979,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -990,7 +993,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>21</v>
@@ -1003,28 +1006,28 @@
       <c r="M11" s="18"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40" t="s">
+      <c r="B12" s="41"/>
+      <c r="C12" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="42"/>
+      <c r="E12" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="41"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="45"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
       <c r="M12" s="18"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1058,109 +1061,109 @@
       <c r="J13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
       <c r="M13" s="18"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="38" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="5">
         <v>8</v>
       </c>
       <c r="C14" s="24">
-        <v>0.18</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D14" s="24">
-        <v>0.19</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="E14" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="F14" s="25">
-        <v>0.215</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="G14" s="24">
-        <v>0.33</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="H14" s="24">
-        <v>0.35</v>
+        <v>0.373</v>
       </c>
       <c r="I14" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.182</v>
       </c>
       <c r="J14" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.222</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="43"/>
+      <c r="L14" s="28"/>
       <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="5">
         <v>13.5</v>
       </c>
       <c r="C15" s="24">
-        <v>0.18</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="D15" s="24">
-        <v>0.19</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="E15" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="F15" s="25">
-        <v>0.215</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="G15" s="24">
-        <v>0.33</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="H15" s="24">
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
       <c r="I15" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="J15" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="43"/>
+      <c r="L15" s="28"/>
       <c r="M15" s="18"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="5">
         <v>16</v>
       </c>
       <c r="C16" s="24">
-        <v>0.18</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="D16" s="24">
-        <v>0.19</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="E16" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="F16" s="25">
-        <v>0.215</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="G16" s="24">
-        <v>0.33</v>
+        <v>0.307</v>
       </c>
       <c r="H16" s="24">
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
       <c r="I16" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="J16" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.437</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="43"/>
+      <c r="L16" s="28"/>
       <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1179,104 +1182,104 @@
       <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="5">
         <v>8</v>
       </c>
       <c r="C18" s="24">
-        <v>0.18</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D18" s="24">
-        <v>0.19</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="E18" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="F18" s="25">
-        <v>0.215</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="G18" s="24">
-        <v>0.33</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="H18" s="24">
-        <v>0.35</v>
+        <v>0.373</v>
       </c>
       <c r="I18" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="J18" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="43"/>
+      <c r="L18" s="28"/>
       <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="5">
         <v>13.5</v>
       </c>
       <c r="C19" s="24">
-        <v>0.18</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="D19" s="24">
-        <v>0.19</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="E19" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="F19" s="25">
-        <v>0.215</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="G19" s="24">
-        <v>0.33</v>
+        <v>0.307</v>
       </c>
       <c r="H19" s="24">
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
       <c r="I19" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="J19" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="43"/>
+      <c r="L19" s="28"/>
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="5">
         <v>16</v>
       </c>
       <c r="C20" s="24">
-        <v>0.18</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="D20" s="24">
-        <v>0.19</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="E20" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.193</v>
       </c>
       <c r="F20" s="25">
-        <v>0.215</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="G20" s="24">
-        <v>0.33</v>
+        <v>0.308</v>
       </c>
       <c r="H20" s="24">
-        <v>0.35</v>
+        <v>0.376</v>
       </c>
       <c r="I20" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="J20" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="43"/>
+      <c r="L20" s="28"/>
       <c r="M20" s="18"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1295,104 +1298,104 @@
       <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="5">
         <v>8</v>
       </c>
       <c r="C22" s="24">
-        <v>0.18</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="D22" s="24">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="E22" s="24">
         <v>0.19</v>
       </c>
-      <c r="E22" s="24">
-        <v>0.20499999999999999</v>
-      </c>
       <c r="F22" s="25">
-        <v>0.215</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="G22" s="24">
-        <v>0.33</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="H22" s="24">
-        <v>0.35</v>
+        <v>0.372</v>
       </c>
       <c r="I22" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="J22" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.21</v>
       </c>
       <c r="K22" s="2"/>
-      <c r="L22" s="43"/>
+      <c r="L22" s="28"/>
       <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="5">
         <v>13.5</v>
       </c>
       <c r="C23" s="24">
-        <v>0.18</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D23" s="24">
-        <v>0.19</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="E23" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="F23" s="25">
-        <v>0.215</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="G23" s="24">
-        <v>0.33</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="H23" s="24">
-        <v>0.35</v>
+        <v>0.373</v>
       </c>
       <c r="I23" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="J23" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="K23" s="2"/>
-      <c r="L23" s="43"/>
+      <c r="L23" s="28"/>
       <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="5">
         <v>16</v>
       </c>
       <c r="C24" s="24">
-        <v>0.18</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="D24" s="24">
-        <v>0.19</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="E24" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="F24" s="25">
-        <v>0.215</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="G24" s="24">
-        <v>0.33</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="H24" s="24">
-        <v>0.35</v>
+        <v>0.374</v>
       </c>
       <c r="I24" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.30199999999999999</v>
       </c>
       <c r="J24" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.37</v>
       </c>
       <c r="K24" s="2"/>
-      <c r="L24" s="43"/>
+      <c r="L24" s="28"/>
       <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1402,108 +1405,108 @@
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
       <c r="K25" s="18"/>
-      <c r="L25" s="44"/>
+      <c r="L25" s="29"/>
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
-        <v>28</v>
+      <c r="A26" s="46" t="s">
+        <v>40</v>
       </c>
       <c r="B26" s="5">
         <v>8</v>
       </c>
       <c r="C26" s="24">
-        <v>0.18</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D26" s="24">
-        <v>0.19</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="E26" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="F26" s="25">
-        <v>0.215</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="G26" s="24">
-        <v>0.33</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="H26" s="24">
-        <v>0.35</v>
+        <v>0.373</v>
       </c>
       <c r="I26" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.182</v>
       </c>
       <c r="J26" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.222</v>
       </c>
       <c r="K26" s="2"/>
-      <c r="L26" s="43"/>
+      <c r="L26" s="28"/>
       <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="5">
         <v>13.5</v>
       </c>
       <c r="C27" s="24">
-        <v>0.18</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="D27" s="24">
-        <v>0.19</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="E27" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="F27" s="25">
-        <v>0.215</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="G27" s="24">
-        <v>0.33</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="H27" s="24">
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
       <c r="I27" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="J27" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="K27" s="2"/>
-      <c r="L27" s="43"/>
+      <c r="L27" s="28"/>
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="5">
         <v>16</v>
       </c>
       <c r="C28" s="24">
-        <v>0.18</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="D28" s="24">
-        <v>0.19</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="E28" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="F28" s="25">
-        <v>0.215</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="G28" s="24">
-        <v>0.33</v>
+        <v>0.307</v>
       </c>
       <c r="H28" s="24">
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
       <c r="I28" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="J28" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.437</v>
       </c>
       <c r="K28" s="2"/>
-      <c r="L28" s="43"/>
+      <c r="L28" s="28"/>
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1513,108 +1516,108 @@
       <c r="I29" s="22"/>
       <c r="J29" s="22"/>
       <c r="K29" s="18"/>
-      <c r="L29" s="44"/>
+      <c r="L29" s="29"/>
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="5">
         <v>8</v>
       </c>
       <c r="C30" s="24">
-        <v>0.18</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="D30" s="24">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="E30" s="24">
         <v>0.19</v>
       </c>
-      <c r="E30" s="24">
-        <v>0.20499999999999999</v>
-      </c>
       <c r="F30" s="25">
-        <v>0.215</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="G30" s="24">
-        <v>0.33</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="H30" s="24">
-        <v>0.35</v>
+        <v>0.372</v>
       </c>
       <c r="I30" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="J30" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.21</v>
       </c>
       <c r="K30" s="2"/>
-      <c r="L30" s="43"/>
+      <c r="L30" s="28"/>
       <c r="M30" s="18"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="5">
         <v>13.5</v>
       </c>
       <c r="C31" s="24">
-        <v>0.18</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D31" s="24">
-        <v>0.19</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="E31" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="F31" s="25">
-        <v>0.215</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="G31" s="24">
-        <v>0.33</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="H31" s="24">
-        <v>0.35</v>
+        <v>0.373</v>
       </c>
       <c r="I31" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="J31" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="K31" s="2"/>
-      <c r="L31" s="43"/>
+      <c r="L31" s="28"/>
       <c r="M31" s="18"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="5">
         <v>16</v>
       </c>
       <c r="C32" s="24">
-        <v>0.18</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="D32" s="24">
-        <v>0.19</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="E32" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="F32" s="25">
-        <v>0.215</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="G32" s="24">
-        <v>0.33</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="H32" s="24">
-        <v>0.35</v>
+        <v>0.374</v>
       </c>
       <c r="I32" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.30199999999999999</v>
       </c>
       <c r="J32" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.37</v>
       </c>
       <c r="K32" s="2"/>
-      <c r="L32" s="43"/>
+      <c r="L32" s="28"/>
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -1623,104 +1626,104 @@
       <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>34</v>
+      <c r="A34" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="B34" s="5">
         <v>8</v>
       </c>
       <c r="C34" s="24">
-        <v>0.18</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="D34" s="24">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="E34" s="24">
         <v>0.19</v>
       </c>
-      <c r="E34" s="24">
-        <v>0.20499999999999999</v>
-      </c>
       <c r="F34" s="25">
-        <v>0.215</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="G34" s="24">
-        <v>0.33</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="H34" s="24">
-        <v>0.35</v>
+        <v>0.372</v>
       </c>
       <c r="I34" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="J34" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.21</v>
       </c>
       <c r="K34" s="2"/>
-      <c r="L34" s="43"/>
+      <c r="L34" s="28"/>
       <c r="M34" s="18"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="5">
         <v>13.5</v>
       </c>
       <c r="C35" s="24">
-        <v>0.18</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D35" s="24">
-        <v>0.19</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="E35" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="F35" s="25">
-        <v>0.215</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="G35" s="24">
-        <v>0.33</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="H35" s="24">
-        <v>0.35</v>
+        <v>0.373</v>
       </c>
       <c r="I35" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="J35" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="K35" s="2"/>
-      <c r="L35" s="43"/>
+      <c r="L35" s="28"/>
       <c r="M35" s="18"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="5">
         <v>16</v>
       </c>
       <c r="C36" s="24">
-        <v>0.18</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="D36" s="24">
-        <v>0.19</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="E36" s="24">
-        <v>0.20499999999999999</v>
+        <v>0.191</v>
       </c>
       <c r="F36" s="25">
-        <v>0.215</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="G36" s="24">
-        <v>0.33</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="H36" s="24">
-        <v>0.35</v>
+        <v>0.374</v>
       </c>
       <c r="I36" s="24">
-        <v>0.19600000000000001</v>
+        <v>0.30199999999999999</v>
       </c>
       <c r="J36" s="24">
-        <v>0.20799999999999999</v>
+        <v>0.37</v>
       </c>
       <c r="K36" s="2"/>
-      <c r="L36" s="43"/>
+      <c r="L36" s="28"/>
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -1730,13 +1733,16 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="K38" s="18"/>
       <c r="L38" s="18"/>
       <c r="M38" s="18"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
       <c r="K39" s="18"/>
       <c r="L39" s="18"/>
       <c r="M39" s="18"/>

</xml_diff>